<commit_message>
Fix some issues with forms
</commit_message>
<xml_diff>
--- a/formshare/tests/resources/forms/case/case_deactivate.xlsx
+++ b/formshare/tests/resources/forms/case/case_deactivate.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" state="visible" r:id="rId2"/>
@@ -165,10 +165,10 @@
     <t xml:space="preserve">form_id</t>
   </si>
   <si>
-    <t xml:space="preserve">Household Exit Survey</t>
-  </si>
-  <si>
-    <t xml:space="preserve">case_deactivate_20210331</t>
+    <t xml:space="preserve">Household Exit Survey – 20230209</t>
+  </si>
+  <si>
+    <t xml:space="preserve">case_deactivate_20230209</t>
   </si>
 </sst>
 </file>
@@ -179,7 +179,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -214,11 +214,6 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -268,7 +263,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -318,10 +313,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -409,10 +400,10 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="246" zoomScaleNormal="246" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.1"/>
@@ -566,8 +557,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -582,13 +573,13 @@
   </sheetPr>
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="246" zoomScaleNormal="246" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="246" zoomScaleNormal="246" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.64"/>
@@ -608,7 +599,7 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="7" t="s">
         <v>33</v>
       </c>
       <c r="B2" s="0" t="n">
@@ -619,7 +610,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="7" t="s">
         <v>33</v>
       </c>
       <c r="B3" s="0" t="n">
@@ -630,7 +621,7 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="7" t="s">
         <v>33</v>
       </c>
       <c r="B4" s="0" t="n">
@@ -641,7 +632,7 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="13" t="s">
         <v>37</v>
       </c>
       <c r="B5" s="0" t="n">
@@ -652,7 +643,7 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="13" t="s">
         <v>37</v>
       </c>
       <c r="B6" s="0" t="n">
@@ -663,7 +654,7 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="13" t="s">
         <v>37</v>
       </c>
       <c r="B7" s="0" t="n">
@@ -674,7 +665,7 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="13" t="s">
         <v>37</v>
       </c>
       <c r="B8" s="0" t="n">
@@ -685,7 +676,7 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="13" t="s">
         <v>37</v>
       </c>
       <c r="B9" s="0" t="n">
@@ -696,7 +687,7 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="13" t="s">
         <v>37</v>
       </c>
       <c r="B10" s="0" t="n">
@@ -707,7 +698,7 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="13" t="s">
         <v>37</v>
       </c>
       <c r="B11" s="0" t="n">
@@ -719,8 +710,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -735,13 +726,13 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="246" zoomScaleNormal="246" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="246" zoomScaleNormal="246" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
   </cols>
@@ -764,8 +755,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
Fix test case ID
</commit_message>
<xml_diff>
--- a/formshare/tests/resources/forms/case/case_deactivate.xlsx
+++ b/formshare/tests/resources/forms/case/case_deactivate.xlsx
@@ -165,10 +165,10 @@
     <t xml:space="preserve">form_id</t>
   </si>
   <si>
-    <t xml:space="preserve">Household Exit Survey – 20230209</t>
-  </si>
-  <si>
-    <t xml:space="preserve">case_deactivate_20230209</t>
+    <t xml:space="preserve">Household Exit Survey – 20210331</t>
+  </si>
+  <si>
+    <t xml:space="preserve">case_deactivate_20210331</t>
   </si>
 </sst>
 </file>
@@ -403,7 +403,7 @@
       <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.1"/>
@@ -579,7 +579,7 @@
       <selection pane="bottomLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.64"/>
@@ -727,12 +727,12 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="246" zoomScaleNormal="246" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
   </cols>

</xml_diff>